<commit_message>
Here is my commit message
</commit_message>
<xml_diff>
--- a/data/data_for_modelling/Codebook_CPI.xlsx
+++ b/data/data_for_modelling/Codebook_CPI.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schwarze/Documents/GitHub/CyberPower/data/data_for_modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBDFF59-AAD6-0E40-8FC8-5F18E3BC4CA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B450B29-1C59-8A49-B8DD-96E421BC3AC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16680" xr2:uid="{9E74F6EE-D43E-CA43-B6F8-4ACE8BB82ECD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="203">
   <si>
     <t>removal_google</t>
   </si>
@@ -223,6 +224,426 @@
   </si>
   <si>
     <t>IH</t>
+  </si>
+  <si>
+    <t>broadband_speed</t>
+  </si>
+  <si>
+    <t>mobile_speed</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Indicator &amp; Definition</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Indicator Construction</t>
+  </si>
+  <si>
+    <t>Cyber related Laws</t>
+  </si>
+  <si>
+    <t>Measurement of how active a country has been in implementing content, privacy, and cyber crime laws</t>
+  </si>
+  <si>
+    <t>Harvard Belfer Cyber Power Project</t>
+  </si>
+  <si>
+    <t>0= no laws; 1= laws that cover one of the following: content, privacy and crime </t>
+  </si>
+  <si>
+    <t>2= laws that cover two of the following: content, privacy and crime</t>
+  </si>
+  <si>
+    <t>3= laws that cover content, privacy and crime, outdated (&lt; yr 2000) </t>
+  </si>
+  <si>
+    <t>4= laws that cover content, privacy and cybersecurity, recent update (&gt;= yr 2000)</t>
+  </si>
+  <si>
+    <t>State-backed Cyber Attacks</t>
+  </si>
+  <si>
+    <t>Number of publicly attributed notably sophisticated cyber attacks</t>
+  </si>
+  <si>
+    <t>CSIS</t>
+  </si>
+  <si>
+    <t>2018/2019</t>
+  </si>
+  <si>
+    <t>Count of cyber attacks attributed to state sponsored actors</t>
+  </si>
+  <si>
+    <t>Bilateral Cyber Agreements</t>
+  </si>
+  <si>
+    <t>Number and quality of bilteral formal and/or informal agreements signed by the national government in cyberspace, scored by recency.</t>
+  </si>
+  <si>
+    <t>For each of the agreements between countries:</t>
+  </si>
+  <si>
+    <t>1 = meeting, remarks</t>
+  </si>
+  <si>
+    <t>2 = Joint Statement, cooperation, framework</t>
+  </si>
+  <si>
+    <t>3 =Agreement / MOU</t>
+  </si>
+  <si>
+    <t>Multilateral Cyber Agreements</t>
+  </si>
+  <si>
+    <t>Number and quality of multilateral formal and/or informal agreements signed by the national government in cyberspace, scored by recency. </t>
+  </si>
+  <si>
+    <t>1 = informal/ conference / regional</t>
+  </si>
+  <si>
+    <t>2 = informal / conference / Global</t>
+  </si>
+  <si>
+    <t>3 = Formal Regional Agreement / Member of Regional Org</t>
+  </si>
+  <si>
+    <t>4 = Formal multilateral Agreement / Member of Global Org</t>
+  </si>
+  <si>
+    <t>Cyber Miltary Doctrine</t>
+  </si>
+  <si>
+    <t>Measurement of existence and quality of cyber military doctrine</t>
+  </si>
+  <si>
+    <t>2010-2018</t>
+  </si>
+  <si>
+    <t>0 = no cyber military strategy</t>
+  </si>
+  <si>
+    <t>1= draft of a cyber military strategy</t>
+  </si>
+  <si>
+    <t>2 = potentially outdated cyber military strategy (5 years or more)</t>
+  </si>
+  <si>
+    <t>3 = new cyber military strategy (less than 5 years) / potentially outdated military strategy but consistently pursued</t>
+  </si>
+  <si>
+    <t>4 = established and refreshed cyber military strategy (strategy less than 5 years old but cyber military strategy consistently followed</t>
+  </si>
+  <si>
+    <t>Global Top 100 Tech Firms</t>
+  </si>
+  <si>
+    <t>Number of Global Top 100 tech firms headquartered in country.</t>
+  </si>
+  <si>
+    <t>Thomson Reuters</t>
+  </si>
+  <si>
+    <t>Count of top tech firms per country</t>
+  </si>
+  <si>
+    <t>High Tech Exports</t>
+  </si>
+  <si>
+    <t>Percentage of high tech exports as total of manufactuing exports</t>
+  </si>
+  <si>
+    <t>World Bank</t>
+  </si>
+  <si>
+    <t>Higher values indicate more technology exports. </t>
+  </si>
+  <si>
+    <t>Human Capital</t>
+  </si>
+  <si>
+    <t>Measurement of how easy it is to find skilled employees in a given country</t>
+  </si>
+  <si>
+    <t>World Economic Forum</t>
+  </si>
+  <si>
+    <t>The measure of interest is based on the question: “In your country, how easy is it for companies to find employees with the required skills for their business needs? (1 = extremely difficult, 7 = extremely easy)”. The measure has subsequently been rescaled to a 100 point scale with high values representing high availability of skilled employees</t>
+  </si>
+  <si>
+    <t>Cyber Military Strategy</t>
+  </si>
+  <si>
+    <t>Cyber Strategies detailing offensive or defensive military capabilities in cyberspace</t>
+  </si>
+  <si>
+    <t>0 = no cyber military strategy </t>
+  </si>
+  <si>
+    <t>4 = established and refreshed cyber military strategy (strategy less than 5 years old but cyber military strategy consistently followed)</t>
+  </si>
+  <si>
+    <t>Centralized Cyber Command</t>
+  </si>
+  <si>
+    <t>The existence and age of a national cyber command.</t>
+  </si>
+  <si>
+    <t>2014- 2020</t>
+  </si>
+  <si>
+    <t>0 = no cyber command</t>
+  </si>
+  <si>
+    <t>1= plans to establish a cyber command </t>
+  </si>
+  <si>
+    <t>2 = new cyber command (less or equal 2 years)</t>
+  </si>
+  <si>
+    <t>3 = established cyber command (2-5 years)</t>
+  </si>
+  <si>
+    <t>4 = established cyber command (more than 5 years) </t>
+  </si>
+  <si>
+    <t>Top Cybersecurity Firms</t>
+  </si>
+  <si>
+    <t>Number of global top cyber security firms headquartered in country</t>
+  </si>
+  <si>
+    <t>Cybersecurity Ventures</t>
+  </si>
+  <si>
+    <t>Number of Top 150 cybersecurity firms listed in the ranking. </t>
+  </si>
+  <si>
+    <t>Computer Infection</t>
+  </si>
+  <si>
+    <t>Percentage of computers in country that are infected with malware</t>
+  </si>
+  <si>
+    <t>Comparitech</t>
+  </si>
+  <si>
+    <t>Q3 2019</t>
+  </si>
+  <si>
+    <t>Percentage of users attacked ( unauthorized access, destruction, disruption) during this period </t>
+  </si>
+  <si>
+    <t>Mobile Infection</t>
+  </si>
+  <si>
+    <t>Percentage of mobiles in country that are infected with malware</t>
+  </si>
+  <si>
+    <t>Social Media Users</t>
+  </si>
+  <si>
+    <t>Percentage of active social media accounts</t>
+  </si>
+  <si>
+    <t>Statista</t>
+  </si>
+  <si>
+    <t>Share of internet users visiting social networking sites. </t>
+  </si>
+  <si>
+    <t>Internet Users</t>
+  </si>
+  <si>
+    <t>Internet penetration rate within a country.</t>
+  </si>
+  <si>
+    <t>2017-2018</t>
+  </si>
+  <si>
+    <t>Higher the more individuals use the internet</t>
+  </si>
+  <si>
+    <t>Surveillance Technology</t>
+  </si>
+  <si>
+    <t>Number of private sector surveillance companies with offices in/ or operating in state</t>
+  </si>
+  <si>
+    <t>Privacy Intenational</t>
+  </si>
+  <si>
+    <t>Count of the number of surveillance companies that operate in a country</t>
+  </si>
+  <si>
+    <t>Top websites</t>
+  </si>
+  <si>
+    <t>Number of websites in the Alexa Top 50 that belong to organizations HQ in that country</t>
+  </si>
+  <si>
+    <t>Alexa</t>
+  </si>
+  <si>
+    <t>Number of sites in the Top 50</t>
+  </si>
+  <si>
+    <t>Top news sites</t>
+  </si>
+  <si>
+    <t>Number of news sites in the Alexa Top 50 that belong to organizations HQ in that country</t>
+  </si>
+  <si>
+    <t>Content Removal Requests</t>
+  </si>
+  <si>
+    <t>Number of takedown requests to Google from a government entity</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>2018-2019</t>
+  </si>
+  <si>
+    <t>Number of requests </t>
+  </si>
+  <si>
+    <t>Freedom on the Net</t>
+  </si>
+  <si>
+    <t>Freedom House's score for how free citizens are online</t>
+  </si>
+  <si>
+    <t>Freedom House &amp; Freedom of the World</t>
+  </si>
+  <si>
+    <t>0-100: 3 separate scores aggregated together:</t>
+  </si>
+  <si>
+    <t>a) obstacles to access</t>
+  </si>
+  <si>
+    <t>b) limits on content</t>
+  </si>
+  <si>
+    <t>c) violations of users rights. </t>
+  </si>
+  <si>
+    <t>For seven countries we used freedom of the World rankings because Freedom House did not have the information. </t>
+  </si>
+  <si>
+    <t>ICT Imports</t>
+  </si>
+  <si>
+    <t>Measurement of information and communications imports as a percentage of total imports.</t>
+  </si>
+  <si>
+    <t>UNCTAD</t>
+  </si>
+  <si>
+    <t>2015-2018</t>
+  </si>
+  <si>
+    <t>More imports = higher score. Per capita measure. </t>
+  </si>
+  <si>
+    <t>Patent Applications</t>
+  </si>
+  <si>
+    <t>Number of domestic patent filings by residents of that country</t>
+  </si>
+  <si>
+    <t>World Development Indicators</t>
+  </si>
+  <si>
+    <t>Number of domestic patent filings (residents only). Per capita measure. </t>
+  </si>
+  <si>
+    <t>Broadband Speed</t>
+  </si>
+  <si>
+    <t>Measurement of broadband speed relevant to the fastest broadband rates in the world</t>
+  </si>
+  <si>
+    <t>Speedtest Global Index</t>
+  </si>
+  <si>
+    <t>10 out of 10 is Singapore which has the highest broadband speed in the world. </t>
+  </si>
+  <si>
+    <t>Mobile Speed</t>
+  </si>
+  <si>
+    <t>Measurement of mobile speed relevant to the fastest mobile rates in the world</t>
+  </si>
+  <si>
+    <t>10 out of 10 is UAE which has the fastest mobile internet in the world. </t>
+  </si>
+  <si>
+    <t>E-Commerce</t>
+  </si>
+  <si>
+    <t>National E-commerce sales as a percentage of GDP</t>
+  </si>
+  <si>
+    <t>2017 and 2020</t>
+  </si>
+  <si>
+    <t>Higher the more e-commerce sales. </t>
+  </si>
+  <si>
+    <t>CSIRT</t>
+  </si>
+  <si>
+    <t>Existence of a Cyber Security Incidence Response Team</t>
+  </si>
+  <si>
+    <t>0 = no response team</t>
+  </si>
+  <si>
+    <t>1= plans to establish a CSIRT</t>
+  </si>
+  <si>
+    <t>2 = new national CSIRT team (less or equal 5 years)</t>
+  </si>
+  <si>
+    <t>3 = established national CSIRT team (more than 5 years)</t>
+  </si>
+  <si>
+    <t>4 = established national CSIRT team (more than 5 years) + member of the first response team</t>
+  </si>
+  <si>
+    <t>Vulnerabilities</t>
+  </si>
+  <si>
+    <t>Cumulative percentage of the vulnerabilities listed for a country's infrastructure in the Shodan database</t>
+  </si>
+  <si>
+    <t>Cumulative percentage of the Shodan search results. </t>
+  </si>
+  <si>
+    <t>Global Soft Power</t>
+  </si>
+  <si>
+    <t>Country scores in the Global Soft Power Index</t>
+  </si>
+  <si>
+    <t>Brand Finance</t>
+  </si>
+  <si>
+    <t>The scores calculated by Brand Finance's was part of their Soft Power index. These same scores were used for the Belfer Cyber Power Index. </t>
   </si>
 </sst>
 </file>
@@ -254,7 +675,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -262,16 +683,172 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,11 +1162,912 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63E30DD-F407-7C45-B3FA-851B30EEE369}">
-  <dimension ref="A1:F21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C147AD-D07A-9A44-8E76-A0B5500F5EDE}">
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="31.33203125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="52.5" style="13" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" style="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="12">
+        <v>2020</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9">
+        <v>2</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>3</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="12">
+        <v>2020</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>4</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="12">
+        <v>2020</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="7"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>5</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="7"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="9">
+        <v>6</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="15">
+        <v>2018</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="9">
+        <v>7</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="15">
+        <v>2018</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="9">
+        <v>8</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="E23" s="15">
+        <v>2019</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>9</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="12">
+        <v>2020</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="7"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <v>10</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="5"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="7"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="9">
+        <v>11</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="E34" s="15">
+        <v>2019</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="9">
+        <v>12</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="9">
+        <v>13</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="9">
+        <v>14</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="E37" s="15">
+        <v>2020</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="9">
+        <v>15</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="9">
+        <v>16</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="E39" s="15">
+        <v>2016</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="9">
+        <v>17</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E40" s="15">
+        <v>2019</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="9">
+        <v>18</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E41" s="15">
+        <v>2019</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>19</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="F42" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="3">
+        <v>20</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="E43" s="12">
+        <v>2019</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="5"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="5"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="5"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="7"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="9">
+        <v>21</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="9">
+        <v>22</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="E49" s="15">
+        <v>2018</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="9">
+        <v>23</v>
+      </c>
+      <c r="B50" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="E50" s="16">
+        <v>43891</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="9">
+        <v>24</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="E51" s="16">
+        <v>43891</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>25</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="F52" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="3">
+        <v>26</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E53" s="12">
+        <v>2020</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="5"/>
+      <c r="B54" s="18"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="5"/>
+      <c r="B55" s="18"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="5"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="7"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="9">
+        <v>27</v>
+      </c>
+      <c r="B58" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E58" s="15">
+        <v>2020</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>28</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="D59" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E59" s="13">
+        <v>2019</v>
+      </c>
+      <c r="F59" t="s">
+        <v>202</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63E30DD-F407-7C45-B3FA-851B30EEE369}">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -886,7 +2364,7 @@
         <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D20" t="s">
         <v>55</v>
@@ -904,6 +2382,16 @@
       </c>
       <c r="D21" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>